<commit_message>
Updated models and new R markdown files
</commit_message>
<xml_diff>
--- a/Model_Summary.xlsx
+++ b/Model_Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Git\tmp\GEO_Class\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA53707-8C1C-4DD5-9D34-32194DF2193C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B9DA53-6620-4526-BFE5-88FA1C91C0AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{BFC57F3C-6BA1-430B-B360-C49D61065541}"/>
+    <workbookView xWindow="-18915" yWindow="2805" windowWidth="15750" windowHeight="11055" xr2:uid="{BFC57F3C-6BA1-430B-B360-C49D61065541}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="20">
   <si>
     <t>Model Type</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Archtype weights as interactions</t>
+  </si>
+  <si>
+    <t>Log(Chl-a(ug)))</t>
   </si>
 </sst>
 </file>
@@ -114,7 +117,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,18 +127,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -170,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -179,9 +170,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -191,15 +179,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -211,35 +193,59 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -558,31 +564,31 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -590,429 +596,429 @@
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="4">
-        <v>0.97809999999999997</v>
-      </c>
-      <c r="E2" s="16">
-        <v>2882</v>
+      <c r="D2" s="3">
+        <v>0.87309999999999999</v>
+      </c>
+      <c r="E2" s="11">
+        <v>4364</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4">
-        <v>0.4884</v>
-      </c>
-      <c r="E3" s="5">
-        <v>3530</v>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="3">
+        <v>0.53669999999999995</v>
+      </c>
+      <c r="E3" s="4">
+        <v>4546</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8">
-        <v>0.61219999999999997</v>
-      </c>
-      <c r="E4" s="9">
-        <v>3101</v>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="6">
+        <v>0.58709999999999996</v>
+      </c>
+      <c r="E4" s="7">
+        <v>4376</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="4">
-        <v>0.9919</v>
-      </c>
-      <c r="E5" s="16">
-        <v>2882</v>
+      <c r="D5" s="3">
+        <v>0.87319999999999998</v>
+      </c>
+      <c r="E5" s="11">
+        <v>4364</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4">
-        <v>0.4844</v>
-      </c>
-      <c r="E6" s="5">
-        <v>3530</v>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="3">
+        <v>0.53669999999999995</v>
+      </c>
+      <c r="E6" s="4">
+        <v>4546</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8">
-        <v>0.61219999999999997</v>
-      </c>
-      <c r="E7" s="9">
-        <v>3101</v>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="6">
+        <v>0.58720000000000006</v>
+      </c>
+      <c r="E7" s="7">
+        <v>4376</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="4">
-        <v>0.63990000000000002</v>
-      </c>
-      <c r="E8" s="16">
-        <v>3826</v>
+      <c r="D8" s="3">
+        <v>0.85880000000000001</v>
+      </c>
+      <c r="E8" s="11">
+        <v>4542</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4">
-        <v>0.48430000000000001</v>
-      </c>
-      <c r="E9" s="5">
-        <v>4313</v>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="3">
+        <v>0.50760000000000005</v>
+      </c>
+      <c r="E9" s="13">
+        <v>4653</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="8">
-        <v>0.60599999999999998</v>
-      </c>
-      <c r="E10" s="9">
-        <v>3899</v>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="6">
+        <v>0.52900000000000003</v>
+      </c>
+      <c r="E10" s="14">
+        <v>4596</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="4">
-        <v>0.95699999999999996</v>
-      </c>
-      <c r="E11" s="16">
-        <v>2097</v>
+      <c r="D11" s="3">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="E11" s="11">
+        <v>4542</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4">
-        <v>0.41439999999999999</v>
-      </c>
-      <c r="E12" s="5">
-        <v>2394</v>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="3">
+        <v>0.50760000000000005</v>
+      </c>
+      <c r="E12" s="4">
+        <v>4653</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="8">
-        <v>0.5534</v>
-      </c>
-      <c r="E13" s="9">
-        <v>2176</v>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="6">
+        <v>0.52900000000000003</v>
+      </c>
+      <c r="E13" s="7">
+        <v>4596</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="11">
-        <v>0.66920000000000002</v>
-      </c>
-      <c r="E14" s="14">
-        <v>2968</v>
+      <c r="D14" s="8">
+        <v>0.88780000000000003</v>
+      </c>
+      <c r="E14" s="12">
+        <v>4114</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="4">
-        <v>0.6008</v>
-      </c>
-      <c r="E15" s="5">
-        <v>3108</v>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="3">
+        <v>0.61670000000000003</v>
+      </c>
+      <c r="E15" s="4">
+        <v>4191</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="8">
-        <v>0.6391</v>
-      </c>
-      <c r="E16" s="15">
-        <v>2964</v>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="6">
+        <v>0.63190000000000002</v>
+      </c>
+      <c r="E16" s="13">
+        <v>4141</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="22">
-        <v>0.95960000000000001</v>
-      </c>
-      <c r="E17" s="23">
-        <v>3581</v>
+      <c r="D17" s="18">
+        <v>0.8165</v>
+      </c>
+      <c r="E17" s="12">
+        <v>4952</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4">
-        <v>0.10580000000000001</v>
-      </c>
-      <c r="E18" s="5">
-        <v>3743</v>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="20">
+        <v>0.25269999999999998</v>
+      </c>
+      <c r="E18" s="21">
+        <v>5308</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="21">
-        <v>0.2203</v>
-      </c>
-      <c r="E19" s="15">
-        <v>3539</v>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="22">
+        <v>0.31619999999999998</v>
+      </c>
+      <c r="E19" s="23">
+        <v>5180</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="11">
-        <v>0.96240000000000003</v>
-      </c>
-      <c r="E20" s="18">
-        <v>3694</v>
+      <c r="C20" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="18">
+        <v>0.99060000000000004</v>
+      </c>
+      <c r="E20" s="12">
+        <v>2989</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="4">
-        <v>0.36170000000000002</v>
-      </c>
-      <c r="E21" s="5">
-        <v>3740</v>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="20">
+        <v>0.4299</v>
+      </c>
+      <c r="E21" s="21">
+        <v>3567</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="8">
-        <v>0.37359999999999999</v>
-      </c>
-      <c r="E22" s="17">
-        <v>3726</v>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="22">
+        <v>0.5353</v>
+      </c>
+      <c r="E22" s="23">
+        <v>3268</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="11">
-        <v>0.84930000000000005</v>
-      </c>
-      <c r="E23" s="18">
-        <v>3732</v>
+      <c r="D23" s="24">
+        <v>0.98970000000000002</v>
+      </c>
+      <c r="E23" s="12">
+        <v>1751</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="4">
-        <v>0.1351</v>
-      </c>
-      <c r="E24" s="5">
-        <v>3774</v>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="25">
+        <v>0.21940000000000001</v>
+      </c>
+      <c r="E24" s="26">
+        <v>2192</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="8">
-        <v>0.17730000000000001</v>
-      </c>
-      <c r="E25" s="9">
-        <v>3745</v>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="27">
+        <v>0.3755</v>
+      </c>
+      <c r="E25" s="23">
+        <v>2015</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="11">
-        <v>0.91469999999999996</v>
-      </c>
-      <c r="E26" s="18">
-        <v>2738</v>
+      <c r="C26" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="24">
+        <v>0.80167600000000006</v>
+      </c>
+      <c r="E26" s="12">
+        <v>2672</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="4">
-        <v>0.29060000000000002</v>
-      </c>
-      <c r="E27" s="5">
-        <v>3433</v>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="25">
+        <v>0.31319999999999998</v>
+      </c>
+      <c r="E27" s="26">
+        <v>2750</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="8">
-        <v>0.48670000000000002</v>
-      </c>
-      <c r="E28" s="19">
-        <v>2932</v>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="27">
+        <v>0.33750000000000002</v>
+      </c>
+      <c r="E28" s="23">
+        <v>2733</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="11">
-        <v>0.99870000000000003</v>
-      </c>
-      <c r="E29" s="20">
-        <v>-66</v>
+      <c r="D29" s="24">
+        <v>0.99880000000000002</v>
+      </c>
+      <c r="E29" s="19">
+        <v>-67</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="4">
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="25">
         <v>0.98760000000000003</v>
       </c>
-      <c r="E30" s="16">
+      <c r="E30" s="11">
         <v>-84</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="8">
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="28">
         <v>0.98580000000000001</v>
       </c>
-      <c r="E31" s="19">
+      <c r="E31" s="23">
         <v>-79</v>
       </c>
     </row>
@@ -1020,24 +1026,24 @@
   <mergeCells count="20">
     <mergeCell ref="B29:B31"/>
     <mergeCell ref="C29:C31"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
     <mergeCell ref="B26:B28"/>
     <mergeCell ref="C26:C28"/>
     <mergeCell ref="B20:B22"/>
     <mergeCell ref="C20:C22"/>
     <mergeCell ref="B23:B25"/>
     <mergeCell ref="C23:C25"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="C14:C16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated code, model summaries
</commit_message>
<xml_diff>
--- a/Model_Summary.xlsx
+++ b/Model_Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Git\tmp\GEO_Class\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B9DA53-6620-4526-BFE5-88FA1C91C0AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5D782D-629A-4CF3-9533-179718EE166E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18915" yWindow="2805" windowWidth="15750" windowHeight="11055" xr2:uid="{BFC57F3C-6BA1-430B-B360-C49D61065541}"/>
+    <workbookView xWindow="8160" yWindow="1605" windowWidth="15750" windowHeight="11055" xr2:uid="{BFC57F3C-6BA1-430B-B360-C49D61065541}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="20">
   <si>
     <t>Model Type</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Log(DOC (mg))</t>
   </si>
   <si>
-    <t>Log(TOC(mg))</t>
-  </si>
-  <si>
     <t>Log(Chl-a(ug))</t>
   </si>
   <si>
@@ -94,6 +91,9 @@
   </si>
   <si>
     <t>Log(Chl-a(ug)))</t>
+  </si>
+  <si>
+    <t>Global Model</t>
   </si>
 </sst>
 </file>
@@ -161,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -169,24 +169,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -199,25 +184,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -232,9 +199,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -244,7 +208,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -561,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{997B5561-4FA5-4758-B9B1-131B958FC30A}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34:E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,474 +564,546 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.87309999999999999</v>
-      </c>
-      <c r="E2" s="11">
-        <v>4364</v>
+      <c r="C2" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="21">
+        <v>0.58928519999999995</v>
+      </c>
+      <c r="E2" s="22">
+        <v>4364.732</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="3">
-        <v>0.53669999999999995</v>
-      </c>
-      <c r="E3" s="4">
-        <v>4546</v>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="1">
+        <v>0.53674069999999996</v>
+      </c>
+      <c r="E3" s="1">
+        <v>4546.4470000000001</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="6">
-        <v>0.58709999999999996</v>
-      </c>
-      <c r="E4" s="7">
-        <v>4376</v>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="1">
+        <v>0.58715490000000004</v>
+      </c>
+      <c r="E4" s="1">
+        <v>4376.9279999999999</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0.87319999999999998</v>
-      </c>
-      <c r="E5" s="11">
-        <v>4364</v>
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="8">
+        <v>0.48299819999999999</v>
+      </c>
+      <c r="E5" s="8">
+        <v>4719.1880000000001</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="20">
+        <v>0.58928519999999995</v>
+      </c>
+      <c r="E6" s="6">
+        <v>4364.732</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="3">
-        <v>0.53669999999999995</v>
-      </c>
-      <c r="E6" s="4">
-        <v>4546</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="6">
-        <v>0.58720000000000006</v>
-      </c>
-      <c r="E7" s="7">
-        <v>4376</v>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="9">
+        <v>0.53674069999999996</v>
+      </c>
+      <c r="E7" s="10">
+        <v>4546.4470000000001</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="9">
+        <v>0.58715490000000004</v>
+      </c>
+      <c r="E8" s="10">
+        <v>4376.9279999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="11">
+        <v>0.48299819999999999</v>
+      </c>
+      <c r="E9" s="19">
+        <v>4719.1880000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0.85880000000000001</v>
-      </c>
-      <c r="E8" s="11">
-        <v>4542</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="3">
-        <v>0.50760000000000005</v>
-      </c>
-      <c r="E9" s="13">
-        <v>4653</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="6">
-        <v>0.52900000000000003</v>
-      </c>
-      <c r="E10" s="14">
-        <v>4596</v>
+      <c r="C10" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="20">
+        <v>0.54357829999999996</v>
+      </c>
+      <c r="E10" s="6">
+        <v>4542.8329999999996</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0.85899999999999999</v>
-      </c>
-      <c r="E11" s="11">
-        <v>4542</v>
+        <v>5</v>
+      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="9">
+        <v>0.50760729999999998</v>
+      </c>
+      <c r="E11" s="10">
+        <v>4653.9620000000004</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="3">
-        <v>0.50760000000000005</v>
-      </c>
-      <c r="E12" s="4">
-        <v>4653</v>
+        <v>6</v>
+      </c>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="9">
+        <v>0.52901900000000002</v>
+      </c>
+      <c r="E12" s="10">
+        <v>4596.9080000000004</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="6">
-        <v>0.52900000000000003</v>
-      </c>
-      <c r="E13" s="7">
-        <v>4596</v>
+      <c r="A13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="11">
+        <v>0.47437629999999997</v>
+      </c>
+      <c r="E13" s="19">
+        <v>4756.1989999999996</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="8">
-        <v>0.88780000000000003</v>
-      </c>
-      <c r="E14" s="12">
-        <v>4114</v>
+        <v>16</v>
+      </c>
+      <c r="D14" s="20">
+        <v>0.54357829999999996</v>
+      </c>
+      <c r="E14" s="6">
+        <v>4542.8329999999996</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="3">
-        <v>0.61670000000000003</v>
-      </c>
-      <c r="E15" s="4">
-        <v>4191</v>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="9">
+        <v>0.50760729999999998</v>
+      </c>
+      <c r="E15" s="10">
+        <v>4653.9620000000004</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="6">
-        <v>0.63190000000000002</v>
-      </c>
-      <c r="E16" s="13">
-        <v>4141</v>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="9">
+        <v>0.52901900000000002</v>
+      </c>
+      <c r="E16" s="10">
+        <v>4596.9080000000004</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="18">
-        <v>0.8165</v>
-      </c>
-      <c r="E17" s="12">
-        <v>4952</v>
+      <c r="A17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="11">
+        <v>0.47437629999999997</v>
+      </c>
+      <c r="E17" s="19">
+        <v>4756.1989999999996</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="23">
+        <v>0.63746020000000003</v>
+      </c>
+      <c r="E18" s="7">
+        <v>4114.2049999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="20">
-        <v>0.25269999999999998</v>
-      </c>
-      <c r="E18" s="21">
-        <v>5308</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="22">
-        <v>0.31619999999999998</v>
-      </c>
-      <c r="E19" s="23">
-        <v>5180</v>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="9">
+        <v>0.61678279999999996</v>
+      </c>
+      <c r="E19" s="10">
+        <v>4191.1260000000002</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="18">
-        <v>0.99060000000000004</v>
-      </c>
-      <c r="E20" s="12">
-        <v>2989</v>
+        <v>6</v>
+      </c>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="9">
+        <v>0.63196640000000004</v>
+      </c>
+      <c r="E20" s="10">
+        <v>4141.7160000000003</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="20">
-        <v>0.4299</v>
-      </c>
-      <c r="E21" s="21">
-        <v>3567</v>
+      <c r="A21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="11">
+        <v>0.59821769999999996</v>
+      </c>
+      <c r="E21" s="10">
+        <v>4263.2150000000001</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="22">
-        <v>0.5353</v>
-      </c>
-      <c r="E22" s="23">
-        <v>3268</v>
+      <c r="A22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="23">
+        <v>0.40598980000000001</v>
+      </c>
+      <c r="E22" s="7">
+        <v>4952.1760000000004</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="24">
-        <v>0.98970000000000002</v>
-      </c>
-      <c r="E23" s="12">
-        <v>1751</v>
+        <v>5</v>
+      </c>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="9">
+        <v>0.25227270000000002</v>
+      </c>
+      <c r="E23" s="10">
+        <v>5308.6189999999997</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="25">
-        <v>0.21940000000000001</v>
-      </c>
-      <c r="E24" s="26">
-        <v>2192</v>
+        <v>6</v>
+      </c>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="9">
+        <v>0.31619520000000001</v>
+      </c>
+      <c r="E24" s="10">
+        <v>5180.2510000000002</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="27">
-        <v>0.3755</v>
-      </c>
-      <c r="E25" s="23">
-        <v>2015</v>
+      <c r="A25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="11">
+        <v>6.0649189999999999E-2</v>
+      </c>
+      <c r="E25" s="12">
+        <v>5669.8389999999999</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>19</v>
-      </c>
       <c r="D26" s="24">
-        <v>0.80167600000000006</v>
-      </c>
-      <c r="E26" s="12">
-        <v>2672</v>
+        <v>0.4395444</v>
+      </c>
+      <c r="E26" s="7">
+        <v>4876.6409999999996</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="25">
-        <v>0.31319999999999998</v>
-      </c>
-      <c r="E27" s="26">
-        <v>2750</v>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="13">
+        <v>0.37075930000000001</v>
+      </c>
+      <c r="E27" s="14">
+        <v>5050.9939999999997</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="27">
-        <v>0.33750000000000002</v>
-      </c>
-      <c r="E28" s="23">
-        <v>2733</v>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="13">
+        <v>0.38336910000000002</v>
+      </c>
+      <c r="E28" s="14">
+        <v>5032.6689999999999</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="24">
-        <v>0.99880000000000002</v>
-      </c>
-      <c r="E29" s="19">
-        <v>-67</v>
+      <c r="A29" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="15">
+        <v>0.26771899999999998</v>
+      </c>
+      <c r="E29" s="12">
+        <v>5290.4250000000002</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="23">
+        <v>0.61187630000000004</v>
+      </c>
+      <c r="E30" s="7">
+        <v>2989.7159999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="25">
-        <v>0.98760000000000003</v>
-      </c>
-      <c r="E30" s="11">
-        <v>-84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="9">
+        <v>0.42994500000000002</v>
+      </c>
+      <c r="E31" s="10">
+        <v>3567.5369999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="28">
-        <v>0.98580000000000001</v>
-      </c>
-      <c r="E31" s="23">
-        <v>-79</v>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="9">
+        <v>0.53534579999999998</v>
+      </c>
+      <c r="E32" s="10">
+        <v>3268.8470000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="11">
+        <v>0.35962880000000003</v>
+      </c>
+      <c r="E33" s="12">
+        <v>3743.386</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="24">
+        <v>0.53850189999999998</v>
+      </c>
+      <c r="E34" s="7">
+        <v>1751.299</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="13">
+        <v>0.21945580000000001</v>
+      </c>
+      <c r="E35" s="14">
+        <v>2192.8209999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="13">
+        <v>0.37553160000000002</v>
+      </c>
+      <c r="E36" s="14">
+        <v>2015.0039999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="15">
+        <v>0.1117469</v>
+      </c>
+      <c r="E37" s="12">
+        <v>2301.8670000000002</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
+  <mergeCells count="18">
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C10:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>